<commit_message>
fixed code to save files to Location Details folder
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,12 +457,12 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Spencer Farm Winery Beer Vs Wine 5k 2021-10-15 22:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: sports</t>
+          <t>Milwaukee Bucks vs Indiana Pacers 2021-10-25 23:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: sports</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Swerve Conference 2021 (In-person) 2021-10-29 12:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: conferences</t>
+          <t>PATINS Access to Education 2021-11-17 14:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: conferences</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lil Inferno 2021-11-11 00:30:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: concerts</t>
+          <t>Passafire and Indubious 2021-11-08 01:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: concerts</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -485,7 +485,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Paranormal Circus - Indianapolis, IN - Friday Oct 29 at 7:30pm 2021-10-29 23:30:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: performing-arts</t>
+          <t>State Ballet of Ukraine: Cinderella 2021-11-17 00:30:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: performing-arts</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -494,10 +494,14 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Major Restaurant</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Good Journeys Expo ‑ Fall 2021-10-23 04:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: festivals</t>
+          <t>The (W)hole in Our HeArts, part of Spirit &amp; Place Festival 2021-11-06 14:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: festivals</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -509,7 +513,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LeadingAge Indiana Fall Conference 2021-09-27 13:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: expos</t>
+          <t>Footnote &amp; Risk Factor Disclosures: Current Examples &amp; Best Practices 2021-11-17 14:00:00+00:00Port-aux-Francais, Kerguelen,  TF.Category: expos</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -520,7 +524,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Burritos &amp; Beer Restaurant, LLC</t>
+          <t>Bluebeard</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -532,7 +536,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10 West Restaurant &amp; Bar</t>
+          <t>Yats</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -540,11 +544,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bluebeard</t>
+          <t>Tinker Street Restaurant</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -552,11 +556,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yats</t>
+          <t>Livery</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -564,11 +568,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tinker Street Restaurant</t>
+          <t>Nesso</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -576,11 +580,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Livery</t>
+          <t>Axum Ethiopian Restaurant</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -588,11 +592,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Axum Ethiopian Restaurant</t>
+          <t>Oakleys Bistro</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -600,11 +604,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A2Z Cafe (Inside and patio dining or Carry-out to Curbside)</t>
+          <t>Mama Carolla's</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -612,27 +616,15 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Slapfish</t>
+          <t>Kuma's Corner</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Mama Carolla's</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>